<commit_message>
Updated with Sami's Order Crossover (Operators Random solutions still being run)
</commit_message>
<xml_diff>
--- a/assignment1/trunk/Operators.xlsx
+++ b/assignment1/trunk/Operators.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12720" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="2060" yWindow="0" windowWidth="34200" windowHeight="23560" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -831,11 +831,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2098553944"/>
-        <c:axId val="-2055170744"/>
+        <c:axId val="-2048160216"/>
+        <c:axId val="-2048157096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2098553944"/>
+        <c:axId val="-2048160216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,7 +845,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2055170744"/>
+        <c:crossAx val="-2048157096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -853,7 +853,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2055170744"/>
+        <c:axId val="-2048157096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,7 +864,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098553944"/>
+        <c:crossAx val="-2048160216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1580,11 +1580,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2057383704"/>
-        <c:axId val="-2062627144"/>
+        <c:axId val="-2048188392"/>
+        <c:axId val="-2048185272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2057383704"/>
+        <c:axId val="-2048188392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1594,7 +1594,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2062627144"/>
+        <c:crossAx val="-2048185272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1602,7 +1602,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2062627144"/>
+        <c:axId val="-2048185272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2057383704"/>
+        <c:crossAx val="-2048188392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2324,11 +2324,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2063520136"/>
-        <c:axId val="-2059790056"/>
+        <c:axId val="-2048429016"/>
+        <c:axId val="-2048425896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2063520136"/>
+        <c:axId val="-2048429016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2338,7 +2338,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059790056"/>
+        <c:crossAx val="-2048425896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2346,7 +2346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2059790056"/>
+        <c:axId val="-2048425896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2357,7 +2357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063520136"/>
+        <c:crossAx val="-2048429016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2472,7 +2472,7 @@
                   <c:v>0.499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55</c:v>
+                  <c:v>0.549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.6</c:v>
@@ -2511,67 +2511,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1424.55089200401</c:v>
+                  <c:v>1432.6282507015</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1442.98993213727</c:v>
+                  <c:v>1980.94314198635</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1419.89715897226</c:v>
+                  <c:v>1797.08682082455</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1415.3727278418</c:v>
+                  <c:v>1699.87024032795</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1434.88262418684</c:v>
+                  <c:v>1664.99558025342</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1424.92215491846</c:v>
+                  <c:v>1619.3175165048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1426.91310421797</c:v>
+                  <c:v>1558.37331595776</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1432.12252560805</c:v>
+                  <c:v>1566.05519733983</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1434.55939997821</c:v>
+                  <c:v>1542.92856037289</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1429.90640133596</c:v>
+                  <c:v>1526.93414356416</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1393.99695396683</c:v>
+                  <c:v>1528.48552183478</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1426.47957756531</c:v>
+                  <c:v>1503.44875279261</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1421.90565739411</c:v>
+                  <c:v>1537.62724071796</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1409.36473089994</c:v>
+                  <c:v>1517.74013126693</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1419.76323158296</c:v>
+                  <c:v>1521.82598689803</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1412.79448727233</c:v>
+                  <c:v>1527.58634403618</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1447.83906253839</c:v>
+                  <c:v>1492.57582897075</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1448.29113700837</c:v>
+                  <c:v>1507.10166655074</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1435.2935240839</c:v>
+                  <c:v>1506.8761306507</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1425.5479132573</c:v>
+                  <c:v>1474.05449482605</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1434.17971437867</c:v>
+                  <c:v>1487.46579561911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2632,7 +2632,7 @@
                   <c:v>0.499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55</c:v>
+                  <c:v>0.549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.6</c:v>
@@ -2671,67 +2671,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1647.65973882359</c:v>
+                  <c:v>1643.72915824597</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1629.13962998908</c:v>
+                  <c:v>1386.50535561005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1639.71952559769</c:v>
+                  <c:v>1145.09210510815</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1651.19303255293</c:v>
+                  <c:v>1059.76021514212</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1630.12999083499</c:v>
+                  <c:v>959.656691047246</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1662.13750823624</c:v>
+                  <c:v>937.594785668093</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1619.93119907089</c:v>
+                  <c:v>848.28958695588</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1640.8185912303</c:v>
+                  <c:v>856.849705579704</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1650.37574662012</c:v>
+                  <c:v>802.184200038888</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1682.96616869961</c:v>
+                  <c:v>734.479094520733</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1681.03901192994</c:v>
+                  <c:v>752.493721998987</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1604.22824507326</c:v>
+                  <c:v>747.191124534011</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1670.08747385978</c:v>
+                  <c:v>740.456819031374</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1649.8449753374</c:v>
+                  <c:v>717.908334752983</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1641.36297949455</c:v>
+                  <c:v>719.659372839877</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1668.95371271326</c:v>
+                  <c:v>705.630455352213</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1678.03222136924</c:v>
+                  <c:v>648.100706597742</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1671.7181281254</c:v>
+                  <c:v>646.666143149707</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1621.32601508592</c:v>
+                  <c:v>679.009157686359</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1662.59574263032</c:v>
+                  <c:v>672.760412320099</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1654.22949867769</c:v>
+                  <c:v>678.439878577821</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2792,7 +2792,7 @@
                   <c:v>0.499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55</c:v>
+                  <c:v>0.549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.6</c:v>
@@ -2831,67 +2831,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1425.81350263455</c:v>
+                  <c:v>1429.33246190672</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1428.91631659722</c:v>
+                  <c:v>1317.38320203548</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1431.68219175238</c:v>
+                  <c:v>1189.81564742232</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1425.19842742671</c:v>
+                  <c:v>1148.88804073035</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1416.15295867923</c:v>
+                  <c:v>975.2161107464231</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1432.03434187396</c:v>
+                  <c:v>945.587066278021</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1420.08859816793</c:v>
+                  <c:v>802.498772981338</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1437.08578716283</c:v>
+                  <c:v>842.658146432476</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1427.03820156566</c:v>
+                  <c:v>814.219709159491</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1412.82147724424</c:v>
+                  <c:v>727.330847689659</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1417.99752428684</c:v>
+                  <c:v>714.373759587404</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1386.67380019021</c:v>
+                  <c:v>732.331261260049</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1429.22365171829</c:v>
+                  <c:v>760.630547869218</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1403.78330431961</c:v>
+                  <c:v>728.68604022727</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1426.87045768297</c:v>
+                  <c:v>657.151402989116</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1430.99238750812</c:v>
+                  <c:v>698.691027682086</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1418.97250159331</c:v>
+                  <c:v>640.500609264187</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1425.77162542391</c:v>
+                  <c:v>671.457618887045</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1422.23882758975</c:v>
+                  <c:v>653.629268924649</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1429.51859239918</c:v>
+                  <c:v>676.138094107391</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1426.49191845612</c:v>
+                  <c:v>624.936566150996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2952,7 +2952,7 @@
                   <c:v>0.499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55</c:v>
+                  <c:v>0.549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.6</c:v>
@@ -2991,67 +2991,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1501.62357193584</c:v>
+                  <c:v>1547.98834850965</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1549.43818991173</c:v>
+                  <c:v>1557.18749036411</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1471.81603858672</c:v>
+                  <c:v>1410.72157688221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1503.76493347971</c:v>
+                  <c:v>1281.42747319029</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1542.12337106262</c:v>
+                  <c:v>1341.8947259579</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1516.03899757454</c:v>
+                  <c:v>956.569488005325</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1450.12293885188</c:v>
+                  <c:v>1382.15785648221</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1539.98016047743</c:v>
+                  <c:v>914.767370801354</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1539.28624344432</c:v>
+                  <c:v>1030.62123220362</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1502.74710142719</c:v>
+                  <c:v>1011.38098009677</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1467.79529643414</c:v>
+                  <c:v>886.776430257461</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1457.05036036058</c:v>
+                  <c:v>1206.73737647636</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1461.12802013321</c:v>
+                  <c:v>1128.46800654512</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1470.17966686177</c:v>
+                  <c:v>808.306405738268</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1538.85316281695</c:v>
+                  <c:v>826.706926439304</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1562.05975033867</c:v>
+                  <c:v>915.0149999014239</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1533.64514242318</c:v>
+                  <c:v>1013.51117438302</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1479.28882324187</c:v>
+                  <c:v>750.871405629934</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1468.22372274987</c:v>
+                  <c:v>925.58359600901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1500.22905070531</c:v>
+                  <c:v>839.161846722266</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1505.81271778506</c:v>
+                  <c:v>1164.84153432639</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3068,11 +3068,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2059706360"/>
-        <c:axId val="-2058606280"/>
+        <c:axId val="-2048014904"/>
+        <c:axId val="-2048011784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2059706360"/>
+        <c:axId val="-2048014904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3082,7 +3082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2058606280"/>
+        <c:crossAx val="-2048011784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3090,7 +3090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2058606280"/>
+        <c:axId val="-2048011784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3101,7 +3101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2059706360"/>
+        <c:crossAx val="-2048014904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3158,7 +3158,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3817,11 +3816,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2052228456"/>
-        <c:axId val="-2052227048"/>
+        <c:axId val="-2047958184"/>
+        <c:axId val="-2047955064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2052228456"/>
+        <c:axId val="-2047958184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3831,7 +3830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2052227048"/>
+        <c:crossAx val="-2047955064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3839,7 +3838,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2052227048"/>
+        <c:axId val="-2047955064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3850,14 +3849,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2052228456"/>
+        <c:crossAx val="-2047958184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4372,7 +4370,7 @@
   <dimension ref="A1:E314"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4475,16 +4473,16 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <v>1424.5508920040099</v>
+        <v>1432.6282507015001</v>
       </c>
       <c r="C14">
-        <v>1647.65973882359</v>
+        <v>1643.72915824597</v>
       </c>
       <c r="D14">
-        <v>1425.8135026345501</v>
+        <v>1429.33246190672</v>
       </c>
       <c r="E14">
-        <v>1501.6235719358399</v>
+        <v>1547.98834850965</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4585,16 +4583,16 @@
         <v>0.05</v>
       </c>
       <c r="B29">
-        <v>1442.98993213727</v>
+        <v>1980.9431419863499</v>
       </c>
       <c r="C29">
-        <v>1629.13962998908</v>
+        <v>1386.5053556100499</v>
       </c>
       <c r="D29">
-        <v>1428.91631659722</v>
+        <v>1317.3832020354801</v>
       </c>
       <c r="E29">
-        <v>1549.43818991173</v>
+        <v>1557.1874903641101</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -4695,16 +4693,16 @@
         <v>0.1</v>
       </c>
       <c r="B44">
-        <v>1419.8971589722601</v>
+        <v>1797.0868208245499</v>
       </c>
       <c r="C44">
-        <v>1639.7195255976901</v>
+        <v>1145.09210510815</v>
       </c>
       <c r="D44">
-        <v>1431.68219175238</v>
+        <v>1189.8156474223199</v>
       </c>
       <c r="E44">
-        <v>1471.81603858672</v>
+        <v>1410.72157688221</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -4805,16 +4803,16 @@
         <v>0.15</v>
       </c>
       <c r="B59">
-        <v>1415.3727278418</v>
+        <v>1699.8702403279499</v>
       </c>
       <c r="C59">
-        <v>1651.1930325529299</v>
+        <v>1059.7602151421199</v>
       </c>
       <c r="D59">
-        <v>1425.1984274267099</v>
+        <v>1148.88804073035</v>
       </c>
       <c r="E59">
-        <v>1503.76493347971</v>
+        <v>1281.4274731902899</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -4915,16 +4913,16 @@
         <v>0.2</v>
       </c>
       <c r="B74">
-        <v>1434.8826241868401</v>
+        <v>1664.99558025342</v>
       </c>
       <c r="C74">
-        <v>1630.1299908349899</v>
+        <v>959.656691047246</v>
       </c>
       <c r="D74">
-        <v>1416.1529586792301</v>
+        <v>975.21611074642306</v>
       </c>
       <c r="E74">
-        <v>1542.12337106262</v>
+        <v>1341.8947259578999</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -5025,16 +5023,16 @@
         <v>0.25</v>
       </c>
       <c r="B89">
-        <v>1424.9221549184599</v>
+        <v>1619.3175165048001</v>
       </c>
       <c r="C89">
-        <v>1662.1375082362399</v>
+        <v>937.59478566809298</v>
       </c>
       <c r="D89">
-        <v>1432.0343418739601</v>
+        <v>945.58706627802098</v>
       </c>
       <c r="E89">
-        <v>1516.03899757454</v>
+        <v>956.56948800532496</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -5135,16 +5133,16 @@
         <v>0.3</v>
       </c>
       <c r="B104">
-        <v>1426.9131042179699</v>
+        <v>1558.37331595776</v>
       </c>
       <c r="C104">
-        <v>1619.93119907089</v>
+        <v>848.28958695588005</v>
       </c>
       <c r="D104">
-        <v>1420.0885981679301</v>
+        <v>802.49877298133799</v>
       </c>
       <c r="E104">
-        <v>1450.12293885188</v>
+        <v>1382.15785648221</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -5245,16 +5243,16 @@
         <v>0.35</v>
       </c>
       <c r="B119">
-        <v>1432.12252560805</v>
+        <v>1566.0551973398301</v>
       </c>
       <c r="C119">
-        <v>1640.8185912302999</v>
+        <v>856.84970557970405</v>
       </c>
       <c r="D119">
-        <v>1437.08578716283</v>
+        <v>842.65814643247597</v>
       </c>
       <c r="E119">
-        <v>1539.98016047743</v>
+        <v>914.76737080135399</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -5355,16 +5353,16 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="B134">
-        <v>1434.55939997821</v>
+        <v>1542.9285603728899</v>
       </c>
       <c r="C134">
-        <v>1650.37574662012</v>
+        <v>802.18420003888798</v>
       </c>
       <c r="D134">
-        <v>1427.0382015656601</v>
+        <v>814.219709159491</v>
       </c>
       <c r="E134">
-        <v>1539.28624344432</v>
+        <v>1030.6212322036199</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -5465,16 +5463,16 @@
         <v>0.44999999999999901</v>
       </c>
       <c r="B149">
-        <v>1429.90640133596</v>
+        <v>1526.93414356416</v>
       </c>
       <c r="C149">
-        <v>1682.9661686996101</v>
+        <v>734.47909452073304</v>
       </c>
       <c r="D149">
-        <v>1412.82147724424</v>
+        <v>727.33084768965898</v>
       </c>
       <c r="E149">
-        <v>1502.74710142719</v>
+        <v>1011.38098009677</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -5575,16 +5573,16 @@
         <v>0.499999999999999</v>
       </c>
       <c r="B164">
-        <v>1393.99695396683</v>
+        <v>1528.48552183478</v>
       </c>
       <c r="C164">
-        <v>1681.03901192994</v>
+        <v>752.49372199898698</v>
       </c>
       <c r="D164">
-        <v>1417.99752428684</v>
+        <v>714.37375958740404</v>
       </c>
       <c r="E164">
-        <v>1467.79529643414</v>
+        <v>886.77643025746102</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -5682,19 +5680,19 @@
     </row>
     <row r="179" spans="1:5">
       <c r="A179">
-        <v>0.55000000000000004</v>
+        <v>0.54999999999999905</v>
       </c>
       <c r="B179">
-        <v>1426.4795775653099</v>
+        <v>1503.4487527926101</v>
       </c>
       <c r="C179">
-        <v>1604.22824507326</v>
+        <v>747.19112453401101</v>
       </c>
       <c r="D179">
-        <v>1386.6738001902099</v>
+        <v>732.33126126004902</v>
       </c>
       <c r="E179">
-        <v>1457.05036036058</v>
+        <v>1206.7373764763599</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -5795,16 +5793,16 @@
         <v>0.6</v>
       </c>
       <c r="B194">
-        <v>1421.90565739411</v>
+        <v>1537.6272407179599</v>
       </c>
       <c r="C194">
-        <v>1670.0874738597799</v>
+        <v>740.45681903137404</v>
       </c>
       <c r="D194">
-        <v>1429.2236517182901</v>
+        <v>760.63054786921805</v>
       </c>
       <c r="E194">
-        <v>1461.1280201332099</v>
+        <v>1128.46800654512</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -5905,16 +5903,16 @@
         <v>0.65</v>
       </c>
       <c r="B209">
-        <v>1409.36473089994</v>
+        <v>1517.7401312669299</v>
       </c>
       <c r="C209">
-        <v>1649.8449753374</v>
+        <v>717.90833475298302</v>
       </c>
       <c r="D209">
-        <v>1403.7833043196099</v>
+        <v>728.68604022727004</v>
       </c>
       <c r="E209">
-        <v>1470.1796668617701</v>
+        <v>808.30640573826804</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -6015,16 +6013,16 @@
         <v>0.7</v>
       </c>
       <c r="B224">
-        <v>1419.7632315829601</v>
+        <v>1521.8259868980299</v>
       </c>
       <c r="C224">
-        <v>1641.36297949455</v>
+        <v>719.65937283987705</v>
       </c>
       <c r="D224">
-        <v>1426.87045768297</v>
+        <v>657.15140298911604</v>
       </c>
       <c r="E224">
-        <v>1538.8531628169501</v>
+        <v>826.70692643930397</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -6125,16 +6123,16 @@
         <v>0.75</v>
       </c>
       <c r="B239">
-        <v>1412.7944872723299</v>
+        <v>1527.58634403618</v>
       </c>
       <c r="C239">
-        <v>1668.9537127132601</v>
+        <v>705.63045535221295</v>
       </c>
       <c r="D239">
-        <v>1430.9923875081199</v>
+        <v>698.69102768208597</v>
       </c>
       <c r="E239">
-        <v>1562.05975033867</v>
+        <v>915.01499990142395</v>
       </c>
     </row>
     <row r="241" spans="1:5">
@@ -6235,16 +6233,16 @@
         <v>0.8</v>
       </c>
       <c r="B254">
-        <v>1447.83906253839</v>
+        <v>1492.5758289707501</v>
       </c>
       <c r="C254">
-        <v>1678.03222136924</v>
+        <v>648.10070659774203</v>
       </c>
       <c r="D254">
-        <v>1418.97250159331</v>
+        <v>640.50060926418701</v>
       </c>
       <c r="E254">
-        <v>1533.64514242318</v>
+        <v>1013.51117438302</v>
       </c>
     </row>
     <row r="256" spans="1:5">
@@ -6345,16 +6343,16 @@
         <v>0.85</v>
       </c>
       <c r="B269">
-        <v>1448.29113700837</v>
+        <v>1507.10166655074</v>
       </c>
       <c r="C269">
-        <v>1671.7181281254</v>
+        <v>646.66614314970695</v>
       </c>
       <c r="D269">
-        <v>1425.7716254239101</v>
+        <v>671.45761888704499</v>
       </c>
       <c r="E269">
-        <v>1479.28882324187</v>
+        <v>750.87140562993397</v>
       </c>
     </row>
     <row r="271" spans="1:5">
@@ -6455,16 +6453,16 @@
         <v>0.9</v>
       </c>
       <c r="B284">
-        <v>1435.2935240838999</v>
+        <v>1506.8761306506999</v>
       </c>
       <c r="C284">
-        <v>1621.3260150859201</v>
+        <v>679.009157686359</v>
       </c>
       <c r="D284">
-        <v>1422.2388275897499</v>
+        <v>653.62926892464895</v>
       </c>
       <c r="E284">
-        <v>1468.2237227498699</v>
+        <v>925.58359600900997</v>
       </c>
     </row>
     <row r="286" spans="1:5">
@@ -6565,16 +6563,16 @@
         <v>0.95</v>
       </c>
       <c r="B299">
-        <v>1425.5479132573</v>
+        <v>1474.0544948260499</v>
       </c>
       <c r="C299">
-        <v>1662.59574263032</v>
+        <v>672.76041232009902</v>
       </c>
       <c r="D299">
-        <v>1429.5185923991801</v>
+        <v>676.138094107391</v>
       </c>
       <c r="E299">
-        <v>1500.2290507053101</v>
+        <v>839.16184672226598</v>
       </c>
     </row>
     <row r="301" spans="1:5">
@@ -6675,16 +6673,16 @@
         <v>1</v>
       </c>
       <c r="B314">
-        <v>1434.17971437867</v>
+        <v>1487.4657956191099</v>
       </c>
       <c r="C314">
-        <v>1654.2294986776899</v>
+        <v>678.43987857782099</v>
       </c>
       <c r="D314">
-        <v>1426.4919184561199</v>
+        <v>624.93656615099599</v>
       </c>
       <c r="E314">
-        <v>1505.8127177850599</v>
+        <v>1164.84153432639</v>
       </c>
     </row>
   </sheetData>
@@ -8202,8 +8200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J64" sqref="J64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8232,19 +8230,19 @@
       </c>
       <c r="B2">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1424.5508920040099</v>
+        <v>1432.6282507015001</v>
       </c>
       <c r="C2">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1647.65973882359</v>
+        <v>1643.72915824597</v>
       </c>
       <c r="D2">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1425.8135026345501</v>
+        <v>1429.33246190672</v>
       </c>
       <c r="E2">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1501.6235719358399</v>
+        <v>1547.98834850965</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -8254,19 +8252,19 @@
       </c>
       <c r="B3">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1442.98993213727</v>
+        <v>1980.9431419863499</v>
       </c>
       <c r="C3">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1629.13962998908</v>
+        <v>1386.5053556100499</v>
       </c>
       <c r="D3">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1428.91631659722</v>
+        <v>1317.3832020354801</v>
       </c>
       <c r="E3">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1549.43818991173</v>
+        <v>1557.1874903641101</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -8276,19 +8274,19 @@
       </c>
       <c r="B4">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1419.8971589722601</v>
+        <v>1797.0868208245499</v>
       </c>
       <c r="C4">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1639.7195255976901</v>
+        <v>1145.09210510815</v>
       </c>
       <c r="D4">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1431.68219175238</v>
+        <v>1189.8156474223199</v>
       </c>
       <c r="E4">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1471.81603858672</v>
+        <v>1410.72157688221</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8298,19 +8296,19 @@
       </c>
       <c r="B5">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1415.3727278418</v>
+        <v>1699.8702403279499</v>
       </c>
       <c r="C5">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1651.1930325529299</v>
+        <v>1059.7602151421199</v>
       </c>
       <c r="D5">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1425.1984274267099</v>
+        <v>1148.88804073035</v>
       </c>
       <c r="E5">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1503.76493347971</v>
+        <v>1281.4274731902899</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -8320,19 +8318,19 @@
       </c>
       <c r="B6">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1434.8826241868401</v>
+        <v>1664.99558025342</v>
       </c>
       <c r="C6">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1630.1299908349899</v>
+        <v>959.656691047246</v>
       </c>
       <c r="D6">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1416.1529586792301</v>
+        <v>975.21611074642306</v>
       </c>
       <c r="E6">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1542.12337106262</v>
+        <v>1341.8947259578999</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -8342,19 +8340,19 @@
       </c>
       <c r="B7">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1424.9221549184599</v>
+        <v>1619.3175165048001</v>
       </c>
       <c r="C7">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1662.1375082362399</v>
+        <v>937.59478566809298</v>
       </c>
       <c r="D7">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1432.0343418739601</v>
+        <v>945.58706627802098</v>
       </c>
       <c r="E7">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1516.03899757454</v>
+        <v>956.56948800532496</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -8364,19 +8362,19 @@
       </c>
       <c r="B8">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1426.9131042179699</v>
+        <v>1558.37331595776</v>
       </c>
       <c r="C8">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1619.93119907089</v>
+        <v>848.28958695588005</v>
       </c>
       <c r="D8">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1420.0885981679301</v>
+        <v>802.49877298133799</v>
       </c>
       <c r="E8">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1450.12293885188</v>
+        <v>1382.15785648221</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -8386,19 +8384,19 @@
       </c>
       <c r="B9">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1432.12252560805</v>
+        <v>1566.0551973398301</v>
       </c>
       <c r="C9">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1640.8185912302999</v>
+        <v>856.84970557970405</v>
       </c>
       <c r="D9">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1437.08578716283</v>
+        <v>842.65814643247597</v>
       </c>
       <c r="E9">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1539.98016047743</v>
+        <v>914.76737080135399</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -8408,19 +8406,19 @@
       </c>
       <c r="B10">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1434.55939997821</v>
+        <v>1542.9285603728899</v>
       </c>
       <c r="C10">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1650.37574662012</v>
+        <v>802.18420003888798</v>
       </c>
       <c r="D10">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1427.0382015656601</v>
+        <v>814.219709159491</v>
       </c>
       <c r="E10">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1539.28624344432</v>
+        <v>1030.6212322036199</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -8430,19 +8428,19 @@
       </c>
       <c r="B11">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1429.90640133596</v>
+        <v>1526.93414356416</v>
       </c>
       <c r="C11">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1682.9661686996101</v>
+        <v>734.47909452073304</v>
       </c>
       <c r="D11">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1412.82147724424</v>
+        <v>727.33084768965898</v>
       </c>
       <c r="E11">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1502.74710142719</v>
+        <v>1011.38098009677</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -8452,41 +8450,41 @@
       </c>
       <c r="B12">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1393.99695396683</v>
+        <v>1528.48552183478</v>
       </c>
       <c r="C12">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1681.03901192994</v>
+        <v>752.49372199898698</v>
       </c>
       <c r="D12">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1417.99752428684</v>
+        <v>714.37375958740404</v>
       </c>
       <c r="E12">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1467.79529643414</v>
+        <v>886.77643025746102</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
         <f ca="1">OFFSET(Operators!$A$14, (ROW()-2)*15,0)</f>
-        <v>0.55000000000000004</v>
+        <v>0.54999999999999905</v>
       </c>
       <c r="B13">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1426.4795775653099</v>
+        <v>1503.4487527926101</v>
       </c>
       <c r="C13">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1604.22824507326</v>
+        <v>747.19112453401101</v>
       </c>
       <c r="D13">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1386.6738001902099</v>
+        <v>732.33126126004902</v>
       </c>
       <c r="E13">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1457.05036036058</v>
+        <v>1206.7373764763599</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -8496,19 +8494,19 @@
       </c>
       <c r="B14">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1421.90565739411</v>
+        <v>1537.6272407179599</v>
       </c>
       <c r="C14">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1670.0874738597799</v>
+        <v>740.45681903137404</v>
       </c>
       <c r="D14">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1429.2236517182901</v>
+        <v>760.63054786921805</v>
       </c>
       <c r="E14">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1461.1280201332099</v>
+        <v>1128.46800654512</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -8518,19 +8516,19 @@
       </c>
       <c r="B15">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1409.36473089994</v>
+        <v>1517.7401312669299</v>
       </c>
       <c r="C15">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1649.8449753374</v>
+        <v>717.90833475298302</v>
       </c>
       <c r="D15">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1403.7833043196099</v>
+        <v>728.68604022727004</v>
       </c>
       <c r="E15">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1470.1796668617701</v>
+        <v>808.30640573826804</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -8540,19 +8538,19 @@
       </c>
       <c r="B16">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1419.7632315829601</v>
+        <v>1521.8259868980299</v>
       </c>
       <c r="C16">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1641.36297949455</v>
+        <v>719.65937283987705</v>
       </c>
       <c r="D16">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1426.87045768297</v>
+        <v>657.15140298911604</v>
       </c>
       <c r="E16">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1538.8531628169501</v>
+        <v>826.70692643930397</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -8562,19 +8560,19 @@
       </c>
       <c r="B17">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1412.7944872723299</v>
+        <v>1527.58634403618</v>
       </c>
       <c r="C17">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1668.9537127132601</v>
+        <v>705.63045535221295</v>
       </c>
       <c r="D17">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1430.9923875081199</v>
+        <v>698.69102768208597</v>
       </c>
       <c r="E17">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1562.05975033867</v>
+        <v>915.01499990142395</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -8584,19 +8582,19 @@
       </c>
       <c r="B18">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1447.83906253839</v>
+        <v>1492.5758289707501</v>
       </c>
       <c r="C18">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1678.03222136924</v>
+        <v>648.10070659774203</v>
       </c>
       <c r="D18">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1418.97250159331</v>
+        <v>640.50060926418701</v>
       </c>
       <c r="E18">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1533.64514242318</v>
+        <v>1013.51117438302</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -8606,19 +8604,19 @@
       </c>
       <c r="B19">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1448.29113700837</v>
+        <v>1507.10166655074</v>
       </c>
       <c r="C19">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1671.7181281254</v>
+        <v>646.66614314970695</v>
       </c>
       <c r="D19">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1425.7716254239101</v>
+        <v>671.45761888704499</v>
       </c>
       <c r="E19">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1479.28882324187</v>
+        <v>750.87140562993397</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -8628,19 +8626,19 @@
       </c>
       <c r="B20">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1435.2935240838999</v>
+        <v>1506.8761306506999</v>
       </c>
       <c r="C20">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1621.3260150859201</v>
+        <v>679.009157686359</v>
       </c>
       <c r="D20">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1422.2388275897499</v>
+        <v>653.62926892464895</v>
       </c>
       <c r="E20">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1468.2237227498699</v>
+        <v>925.58359600900997</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -8650,19 +8648,19 @@
       </c>
       <c r="B21">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1425.5479132573</v>
+        <v>1474.0544948260499</v>
       </c>
       <c r="C21">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1662.59574263032</v>
+        <v>672.76041232009902</v>
       </c>
       <c r="D21">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1429.5185923991801</v>
+        <v>676.138094107391</v>
       </c>
       <c r="E21">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1500.2290507053101</v>
+        <v>839.16184672226598</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -8672,19 +8670,19 @@
       </c>
       <c r="B22">
         <f ca="1">OFFSET(Operators!$B$14, (ROW()-2)*15,0)</f>
-        <v>1434.17971437867</v>
+        <v>1487.4657956191099</v>
       </c>
       <c r="C22">
         <f ca="1">OFFSET(Operators!$C$14, (ROW()-2)*15,0)</f>
-        <v>1654.2294986776899</v>
+        <v>678.43987857782099</v>
       </c>
       <c r="D22">
         <f ca="1">OFFSET(Operators!$D$14, (ROW()-2)*15,0)</f>
-        <v>1426.4919184561199</v>
+        <v>624.93656615099599</v>
       </c>
       <c r="E22">
         <f ca="1">OFFSET(Operators!$E$14, (ROW()-2)*15,0)</f>
-        <v>1505.8127177850599</v>
+        <v>1164.84153432639</v>
       </c>
     </row>
   </sheetData>
@@ -8702,7 +8700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>

</xml_diff>